<commit_message>
Fixed typo in the spreadsheet.
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsms9gep/Library/Mobile Documents/com~apple~CloudDocs/MyelinLiteratureRev/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsms9gep/Documents/Papers/MyelinMetaAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A9309B-8F33-6E4A-B883-9FA034DF8445}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A3C3734-9047-374F-A17B-A291CA3F6D0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="880" windowWidth="27640" windowHeight="15960" xr2:uid="{CC79BDAF-19EC-D540-9290-FB0138332C09}"/>
   </bookViews>
@@ -406,9 +406,6 @@
     <t>Harkins</t>
   </si>
   <si>
-    <t>Edema - Hexaclorophene</t>
-  </si>
-  <si>
     <t>0/9</t>
   </si>
   <si>
@@ -1145,13 +1142,16 @@
   </si>
   <si>
     <t>Diffusion, Magnetization transfer, T2 relaxometry, Other</t>
+  </si>
+  <si>
+    <t>Edema - Hexachlorophene</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1533,11 +1533,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F2F701-A91A-FF4F-AECB-41DB57EF7E72}">
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" customWidth="1"/>
@@ -1557,7 +1557,7 @@
     <col min="19" max="19" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1616,9 +1616,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1627,7 +1627,7 @@
         <v>2004</v>
       </c>
       <c r="D2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E2">
         <v>1.5</v>
@@ -1675,7 +1675,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1686,13 +1686,13 @@
         <v>2005</v>
       </c>
       <c r="D3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E3">
         <v>1.5</v>
       </c>
       <c r="F3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G3" t="s">
         <v>105</v>
@@ -1734,24 +1734,24 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" t="s">
         <v>153</v>
-      </c>
-      <c r="B4" t="s">
-        <v>154</v>
       </c>
       <c r="C4">
         <v>2005</v>
       </c>
       <c r="D4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E4">
         <v>1.5</v>
       </c>
       <c r="F4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G4" t="s">
         <v>105</v>
@@ -1790,10 +1790,10 @@
         <v>59</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>2006</v>
       </c>
       <c r="D5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E5">
         <v>1.5</v>
@@ -1852,7 +1852,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1863,13 +1863,13 @@
         <v>2007</v>
       </c>
       <c r="D6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E6">
         <v>1.5</v>
       </c>
       <c r="F6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G6" t="s">
         <v>32</v>
@@ -1911,7 +1911,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -1970,12 +1970,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C8">
         <v>2008</v>
@@ -1990,7 +1990,7 @@
         <v>73</v>
       </c>
       <c r="G8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H8" t="s">
         <v>38</v>
@@ -2014,7 +2014,7 @@
         <v>36</v>
       </c>
       <c r="O8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P8">
         <v>1</v>
@@ -2026,10 +2026,10 @@
         <v>59</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>2008</v>
       </c>
       <c r="D9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -2088,7 +2088,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>2008</v>
       </c>
       <c r="D10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E10">
         <v>7</v>
@@ -2147,7 +2147,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>79</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>2008</v>
       </c>
       <c r="D11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E11">
         <v>1.5</v>
@@ -2203,10 +2203,10 @@
         <v>60</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>84</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>2008</v>
       </c>
       <c r="D12" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E12">
         <v>4.7</v>
@@ -2265,7 +2265,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>88</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>2008</v>
       </c>
       <c r="D13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E13">
         <v>9.4</v>
@@ -2324,7 +2324,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>92</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>98</v>
       </c>
@@ -2442,12 +2442,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B16" t="s">
         <v>269</v>
-      </c>
-      <c r="B16" t="s">
-        <v>270</v>
       </c>
       <c r="C16">
         <v>2009</v>
@@ -2477,7 +2477,7 @@
         <v>15</v>
       </c>
       <c r="L16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="M16" t="s">
         <v>34</v>
@@ -2486,7 +2486,7 @@
         <v>28</v>
       </c>
       <c r="O16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P16">
         <v>2</v>
@@ -2498,12 +2498,12 @@
         <v>60</v>
       </c>
       <c r="S16" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>273</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19">
-      <c r="A17" s="1" t="s">
-        <v>274</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
@@ -2512,13 +2512,13 @@
         <v>2010</v>
       </c>
       <c r="D17" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E17">
         <v>9.4</v>
       </c>
       <c r="F17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G17" t="s">
         <v>32</v>
@@ -2536,7 +2536,7 @@
         <v>33</v>
       </c>
       <c r="L17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M17" t="s">
         <v>82</v>
@@ -2557,10 +2557,10 @@
         <v>60</v>
       </c>
       <c r="S17" s="4" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>107</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>2011</v>
       </c>
       <c r="D18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E18">
         <v>9.4</v>
@@ -2595,7 +2595,7 @@
         <v>33</v>
       </c>
       <c r="L18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M18" t="s">
         <v>82</v>
@@ -2619,9 +2619,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -2630,7 +2630,7 @@
         <v>2011</v>
       </c>
       <c r="D19" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E19">
         <v>1.5</v>
@@ -2663,7 +2663,7 @@
         <v>9</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P19" t="s">
         <v>42</v>
@@ -2675,21 +2675,21 @@
         <v>60</v>
       </c>
       <c r="S19" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="20" spans="1:19">
-      <c r="A20" s="1" t="s">
+      <c r="B20" t="s">
         <v>281</v>
-      </c>
-      <c r="B20" t="s">
-        <v>282</v>
       </c>
       <c r="C20">
         <v>2011</v>
       </c>
       <c r="D20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E20">
         <v>3</v>
@@ -2713,7 +2713,7 @@
         <v>33</v>
       </c>
       <c r="L20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="M20" t="s">
         <v>34</v>
@@ -2722,7 +2722,7 @@
         <v>1</v>
       </c>
       <c r="O20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P20">
         <v>9</v>
@@ -2734,10 +2734,10 @@
         <v>59</v>
       </c>
       <c r="S20" s="4" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>109</v>
       </c>
@@ -2796,24 +2796,24 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B22" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C22">
         <v>2012</v>
       </c>
       <c r="D22" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E22">
         <v>3</v>
       </c>
       <c r="F22" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G22" t="s">
         <v>55</v>
@@ -2831,7 +2831,7 @@
         <v>33</v>
       </c>
       <c r="L22" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M22" t="s">
         <v>17</v>
@@ -2840,7 +2840,7 @@
         <v>1</v>
       </c>
       <c r="O22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P22">
         <v>18</v>
@@ -2852,10 +2852,10 @@
         <v>60</v>
       </c>
       <c r="S22" s="4" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>115</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>2013</v>
       </c>
       <c r="D23" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E23">
         <v>7</v>
@@ -2914,7 +2914,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>120</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>2013</v>
       </c>
       <c r="D24" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E24">
         <v>9.4</v>
@@ -2943,7 +2943,7 @@
         <v>47</v>
       </c>
       <c r="J24" t="s">
-        <v>122</v>
+        <v>368</v>
       </c>
       <c r="K24" t="s">
         <v>15</v>
@@ -2958,7 +2958,7 @@
         <v>9</v>
       </c>
       <c r="O24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P24">
         <v>4</v>
@@ -2970,27 +2970,27 @@
         <v>59</v>
       </c>
       <c r="S24" s="4" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C25">
         <v>2013</v>
       </c>
       <c r="D25" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E25">
         <v>9.4</v>
       </c>
       <c r="F25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G25" t="s">
         <v>32</v>
@@ -3002,7 +3002,7 @@
         <v>47</v>
       </c>
       <c r="J25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K25" t="s">
         <v>33</v>
@@ -3029,27 +3029,27 @@
         <v>59</v>
       </c>
       <c r="S25" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" t="s">
         <v>128</v>
-      </c>
-      <c r="B26" t="s">
-        <v>129</v>
       </c>
       <c r="C26">
         <v>2013</v>
       </c>
       <c r="D26" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E26">
         <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G26" t="s">
         <v>95</v>
@@ -3076,7 +3076,7 @@
         <v>10</v>
       </c>
       <c r="O26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P26">
         <v>1</v>
@@ -3088,12 +3088,12 @@
         <v>59</v>
       </c>
       <c r="S26" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B27" t="s">
         <v>11</v>
@@ -3102,7 +3102,7 @@
         <v>2014</v>
       </c>
       <c r="D27" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E27">
         <v>7</v>
@@ -3147,12 +3147,12 @@
         <v>60</v>
       </c>
       <c r="S27" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19">
-      <c r="A28" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="B28" t="s">
         <v>99</v>
@@ -3167,7 +3167,7 @@
         <v>4.7</v>
       </c>
       <c r="F28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G28" t="s">
         <v>55</v>
@@ -3179,7 +3179,7 @@
         <v>48</v>
       </c>
       <c r="J28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K28" t="s">
         <v>15</v>
@@ -3206,12 +3206,12 @@
         <v>59</v>
       </c>
       <c r="S28" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B29" t="s">
         <v>116</v>
@@ -3220,7 +3220,7 @@
         <v>2015</v>
       </c>
       <c r="D29" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E29">
         <v>7</v>
@@ -3238,7 +3238,7 @@
         <v>48</v>
       </c>
       <c r="J29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K29" t="s">
         <v>33</v>
@@ -3253,7 +3253,7 @@
         <v>24</v>
       </c>
       <c r="O29" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="P29">
         <v>1</v>
@@ -3265,15 +3265,15 @@
         <v>59</v>
       </c>
       <c r="S29" s="4" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B30" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C30">
         <v>2015</v>
@@ -3285,10 +3285,10 @@
         <v>9.4</v>
       </c>
       <c r="F30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G30" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H30" t="s">
         <v>77</v>
@@ -3312,7 +3312,7 @@
         <v>1</v>
       </c>
       <c r="O30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P30">
         <v>965</v>
@@ -3324,21 +3324,21 @@
         <v>59</v>
       </c>
       <c r="S30" s="4" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B31" t="s">
         <v>158</v>
-      </c>
-      <c r="B31" t="s">
-        <v>159</v>
       </c>
       <c r="C31">
         <v>2015</v>
       </c>
       <c r="D31" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E31">
         <v>7</v>
@@ -3371,7 +3371,7 @@
         <v>15</v>
       </c>
       <c r="O31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P31">
         <v>1</v>
@@ -3383,12 +3383,12 @@
         <v>59</v>
       </c>
       <c r="S31" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B32" t="s">
         <v>99</v>
@@ -3403,7 +3403,7 @@
         <v>4.7</v>
       </c>
       <c r="F32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G32" t="s">
         <v>32</v>
@@ -3442,15 +3442,15 @@
         <v>60</v>
       </c>
       <c r="S32" s="4" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B33" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C33">
         <v>2016</v>
@@ -3462,7 +3462,7 @@
         <v>7</v>
       </c>
       <c r="F33" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G33" t="s">
         <v>55</v>
@@ -3474,7 +3474,7 @@
         <v>47</v>
       </c>
       <c r="J33" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K33" t="s">
         <v>33</v>
@@ -3501,30 +3501,30 @@
         <v>59</v>
       </c>
       <c r="S33" s="4" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C34">
         <v>2016</v>
       </c>
       <c r="D34" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E34">
         <v>9.4</v>
       </c>
       <c r="F34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H34" t="s">
         <v>77</v>
@@ -3539,7 +3539,7 @@
         <v>33</v>
       </c>
       <c r="L34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M34" t="s">
         <v>82</v>
@@ -3548,7 +3548,7 @@
         <v>5</v>
       </c>
       <c r="O34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P34">
         <v>12</v>
@@ -3560,30 +3560,30 @@
         <v>59</v>
       </c>
       <c r="S34" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="35" spans="1:19">
-      <c r="A35" s="1" t="s">
+      <c r="B35" t="s">
         <v>173</v>
-      </c>
-      <c r="B35" t="s">
-        <v>174</v>
       </c>
       <c r="C35">
         <v>2016</v>
       </c>
       <c r="D35" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E35">
         <v>7</v>
       </c>
       <c r="F35" t="s">
+        <v>174</v>
+      </c>
+      <c r="G35" t="s">
         <v>175</v>
-      </c>
-      <c r="G35" t="s">
-        <v>176</v>
       </c>
       <c r="H35" t="s">
         <v>38</v>
@@ -3607,7 +3607,7 @@
         <v>21</v>
       </c>
       <c r="O35" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="P35">
         <v>1</v>
@@ -3619,15 +3619,15 @@
         <v>59</v>
       </c>
       <c r="S35" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="36" spans="1:19">
-      <c r="A36" s="1" t="s">
+      <c r="B36" t="s">
         <v>179</v>
-      </c>
-      <c r="B36" t="s">
-        <v>180</v>
       </c>
       <c r="C36">
         <v>2016</v>
@@ -3639,10 +3639,10 @@
         <v>15.2</v>
       </c>
       <c r="F36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H36" t="s">
         <v>77</v>
@@ -3651,13 +3651,13 @@
         <v>48</v>
       </c>
       <c r="J36" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K36" t="s">
         <v>33</v>
       </c>
       <c r="L36" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M36" t="s">
         <v>34</v>
@@ -3678,27 +3678,27 @@
         <v>59</v>
       </c>
       <c r="S36" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="37" spans="1:19">
-      <c r="A37" s="1" t="s">
+      <c r="B37" t="s">
         <v>184</v>
-      </c>
-      <c r="B37" t="s">
-        <v>185</v>
       </c>
       <c r="C37">
         <v>2016</v>
       </c>
       <c r="D37" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E37">
         <v>9.4</v>
       </c>
       <c r="F37" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G37" t="s">
         <v>55</v>
@@ -3710,7 +3710,7 @@
         <v>13</v>
       </c>
       <c r="J37" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K37" t="s">
         <v>33</v>
@@ -3725,7 +3725,7 @@
         <v>13</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="P37">
         <v>3</v>
@@ -3737,27 +3737,27 @@
         <v>59</v>
       </c>
       <c r="S37" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="38" spans="1:19">
-      <c r="A38" s="1" t="s">
+      <c r="B38" t="s">
         <v>190</v>
-      </c>
-      <c r="B38" t="s">
-        <v>191</v>
       </c>
       <c r="C38">
         <v>2016</v>
       </c>
       <c r="D38" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E38">
         <v>7</v>
       </c>
       <c r="F38" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G38" t="s">
         <v>55</v>
@@ -3769,7 +3769,7 @@
         <v>47</v>
       </c>
       <c r="J38" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K38" t="s">
         <v>33</v>
@@ -3784,7 +3784,7 @@
         <v>25</v>
       </c>
       <c r="O38" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P38">
         <v>1</v>
@@ -3796,15 +3796,15 @@
         <v>59</v>
       </c>
       <c r="S38" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B39" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C39">
         <v>2017</v>
@@ -3816,7 +3816,7 @@
         <v>11.7</v>
       </c>
       <c r="F39" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G39" t="s">
         <v>55</v>
@@ -3834,7 +3834,7 @@
         <v>33</v>
       </c>
       <c r="L39" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="M39" t="s">
         <v>17</v>
@@ -3855,21 +3855,21 @@
         <v>59</v>
       </c>
       <c r="S39" s="4" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B40" t="s">
         <v>196</v>
-      </c>
-      <c r="B40" t="s">
-        <v>197</v>
       </c>
       <c r="C40">
         <v>2017</v>
       </c>
       <c r="D40" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E40">
         <v>7</v>
@@ -3878,7 +3878,7 @@
         <v>45</v>
       </c>
       <c r="G40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H40" t="s">
         <v>77</v>
@@ -3902,7 +3902,7 @@
         <v>14</v>
       </c>
       <c r="O40" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P40">
         <v>1</v>
@@ -3914,21 +3914,21 @@
         <v>59</v>
       </c>
       <c r="S40" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="41" spans="1:19">
-      <c r="A41" s="1" t="s">
+      <c r="B41" t="s">
         <v>200</v>
-      </c>
-      <c r="B41" t="s">
-        <v>201</v>
       </c>
       <c r="C41">
         <v>2017</v>
       </c>
       <c r="D41" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E41">
         <v>11.7</v>
@@ -3952,7 +3952,7 @@
         <v>33</v>
       </c>
       <c r="L41" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M41" t="s">
         <v>82</v>
@@ -3961,7 +3961,7 @@
         <v>14</v>
       </c>
       <c r="O41" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P41">
         <v>8</v>
@@ -3973,30 +3973,30 @@
         <v>59</v>
       </c>
       <c r="S41" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="42" spans="1:19">
-      <c r="A42" s="1" t="s">
+      <c r="B42" t="s">
         <v>204</v>
-      </c>
-      <c r="B42" t="s">
-        <v>205</v>
       </c>
       <c r="C42">
         <v>2017</v>
       </c>
       <c r="D42" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E42">
         <v>7</v>
       </c>
       <c r="F42" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H42" t="s">
         <v>38</v>
@@ -4005,13 +4005,13 @@
         <v>47</v>
       </c>
       <c r="J42" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K42" t="s">
         <v>33</v>
       </c>
       <c r="L42" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M42" t="s">
         <v>34</v>
@@ -4020,7 +4020,7 @@
         <v>20</v>
       </c>
       <c r="O42" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="P42">
         <v>4</v>
@@ -4032,21 +4032,21 @@
         <v>59</v>
       </c>
       <c r="S42" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="43" spans="1:19">
-      <c r="A43" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="B43" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C43">
         <v>2017</v>
       </c>
       <c r="D43" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E43">
         <v>9.4</v>
@@ -4055,7 +4055,7 @@
         <v>37</v>
       </c>
       <c r="G43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H43" t="s">
         <v>78</v>
@@ -4064,13 +4064,13 @@
         <v>47</v>
       </c>
       <c r="J43" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K43" t="s">
         <v>33</v>
       </c>
       <c r="L43" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M43" t="s">
         <v>34</v>
@@ -4079,7 +4079,7 @@
         <v>2</v>
       </c>
       <c r="O43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P43">
         <v>16</v>
@@ -4091,15 +4091,15 @@
         <v>59</v>
       </c>
       <c r="S43" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B44" t="s">
         <v>300</v>
-      </c>
-      <c r="B44" t="s">
-        <v>301</v>
       </c>
       <c r="C44">
         <v>2017</v>
@@ -4123,13 +4123,13 @@
         <v>47</v>
       </c>
       <c r="J44" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K44" t="s">
         <v>33</v>
       </c>
       <c r="L44" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M44" t="s">
         <v>82</v>
@@ -4150,21 +4150,21 @@
         <v>59</v>
       </c>
       <c r="S44" s="4" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B45" t="s">
         <v>214</v>
-      </c>
-      <c r="B45" t="s">
-        <v>215</v>
       </c>
       <c r="C45">
         <v>2018</v>
       </c>
       <c r="D45" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E45">
         <v>7</v>
@@ -4188,7 +4188,7 @@
         <v>33</v>
       </c>
       <c r="L45" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M45" t="s">
         <v>34</v>
@@ -4209,30 +4209,30 @@
         <v>59</v>
       </c>
       <c r="S45" s="4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B46" t="s">
         <v>219</v>
-      </c>
-      <c r="B46" t="s">
-        <v>220</v>
       </c>
       <c r="C46">
         <v>2018</v>
       </c>
       <c r="D46" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E46">
         <v>15.2</v>
       </c>
       <c r="F46" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G46" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H46" t="s">
         <v>77</v>
@@ -4241,7 +4241,7 @@
         <v>48</v>
       </c>
       <c r="J46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K46" t="s">
         <v>33</v>
@@ -4268,45 +4268,45 @@
         <v>59</v>
       </c>
       <c r="S46" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B47" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C47">
         <v>2018</v>
       </c>
       <c r="D47" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E47">
         <v>7</v>
       </c>
       <c r="F47" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G47" t="s">
         <v>32</v>
       </c>
       <c r="H47" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I47" t="s">
         <v>13</v>
       </c>
       <c r="J47" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K47" t="s">
         <v>33</v>
       </c>
       <c r="L47" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M47" t="s">
         <v>34</v>
@@ -4315,7 +4315,7 @@
         <v>6</v>
       </c>
       <c r="O47" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P47">
         <v>79</v>
@@ -4327,15 +4327,15 @@
         <v>60</v>
       </c>
       <c r="S47" s="4" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C48">
         <v>2018</v>
@@ -4347,7 +4347,7 @@
         <v>7</v>
       </c>
       <c r="F48" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G48" t="s">
         <v>55</v>
@@ -4359,13 +4359,13 @@
         <v>48</v>
       </c>
       <c r="J48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K48" t="s">
         <v>33</v>
       </c>
       <c r="L48" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M48" t="s">
         <v>34</v>
@@ -4374,7 +4374,7 @@
         <v>42</v>
       </c>
       <c r="O48" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="P48">
         <v>1</v>
@@ -4386,15 +4386,15 @@
         <v>59</v>
       </c>
       <c r="S48" s="4" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B49" t="s">
         <v>310</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19">
-      <c r="A49" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="B49" t="s">
-        <v>311</v>
       </c>
       <c r="C49">
         <v>2018</v>
@@ -4406,7 +4406,7 @@
         <v>9.4</v>
       </c>
       <c r="F49" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G49" t="s">
         <v>55</v>
@@ -4418,7 +4418,7 @@
         <v>48</v>
       </c>
       <c r="J49" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K49" t="s">
         <v>33</v>
@@ -4445,30 +4445,30 @@
         <v>59</v>
       </c>
       <c r="S49" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C50">
         <v>2018</v>
       </c>
       <c r="D50" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E50">
         <v>15.2</v>
       </c>
       <c r="F50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G50" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H50" t="s">
         <v>77</v>
@@ -4477,13 +4477,13 @@
         <v>48</v>
       </c>
       <c r="J50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K50" t="s">
         <v>33</v>
       </c>
       <c r="L50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M50" t="s">
         <v>82</v>
@@ -4504,15 +4504,15 @@
         <v>59</v>
       </c>
       <c r="S50" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="51" spans="1:19">
-      <c r="A51" s="1" t="s">
+      <c r="B51" t="s">
         <v>229</v>
-      </c>
-      <c r="B51" t="s">
-        <v>230</v>
       </c>
       <c r="C51">
         <v>2018</v>
@@ -4524,7 +4524,7 @@
         <v>7</v>
       </c>
       <c r="F51" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G51" t="s">
         <v>117</v>
@@ -4551,7 +4551,7 @@
         <v>21</v>
       </c>
       <c r="O51" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P51">
         <v>1</v>
@@ -4563,15 +4563,15 @@
         <v>59</v>
       </c>
       <c r="S51" s="4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B52" t="s">
         <v>231</v>
-      </c>
-      <c r="B52" t="s">
-        <v>232</v>
       </c>
       <c r="C52">
         <v>2019</v>
@@ -4583,10 +4583,10 @@
         <v>7</v>
       </c>
       <c r="F52" t="s">
+        <v>236</v>
+      </c>
+      <c r="G52" t="s">
         <v>237</v>
-      </c>
-      <c r="G52" t="s">
-        <v>238</v>
       </c>
       <c r="H52" t="s">
         <v>77</v>
@@ -4595,13 +4595,13 @@
         <v>48</v>
       </c>
       <c r="J52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K52" t="s">
         <v>33</v>
       </c>
       <c r="L52" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M52" t="s">
         <v>34</v>
@@ -4610,7 +4610,7 @@
         <v>5</v>
       </c>
       <c r="O52" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P52">
         <v>12</v>
@@ -4622,30 +4622,30 @@
         <v>60</v>
       </c>
       <c r="S52" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="53" spans="1:19">
-      <c r="A53" s="1" t="s">
+      <c r="B53" t="s">
         <v>242</v>
-      </c>
-      <c r="B53" t="s">
-        <v>243</v>
       </c>
       <c r="C53">
         <v>2019</v>
       </c>
       <c r="D53" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E53">
         <v>11.75</v>
       </c>
       <c r="F53" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G53" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H53" t="s">
         <v>38</v>
@@ -4660,7 +4660,7 @@
         <v>33</v>
       </c>
       <c r="L53" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M53" t="s">
         <v>82</v>
@@ -4669,7 +4669,7 @@
         <v>3</v>
       </c>
       <c r="O53" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P53">
         <v>7</v>
@@ -4681,21 +4681,21 @@
         <v>59</v>
       </c>
       <c r="S53" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B54" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C54">
         <v>2019</v>
       </c>
       <c r="D54" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E54">
         <v>11.7</v>
@@ -4728,7 +4728,7 @@
         <v>13</v>
       </c>
       <c r="O54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="P54">
         <v>1</v>
@@ -4740,15 +4740,15 @@
         <v>59</v>
       </c>
       <c r="S54" s="4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="55" spans="1:19">
-      <c r="A55" s="1" t="s">
+      <c r="B55" t="s">
         <v>321</v>
-      </c>
-      <c r="B55" t="s">
-        <v>322</v>
       </c>
       <c r="C55">
         <v>2019</v>
@@ -4772,13 +4772,13 @@
         <v>13</v>
       </c>
       <c r="J55" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K55" t="s">
         <v>33</v>
       </c>
       <c r="L55" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M55" t="s">
         <v>34</v>
@@ -4799,15 +4799,15 @@
         <v>59</v>
       </c>
       <c r="S55" s="4" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B56" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C56">
         <v>2019</v>
@@ -4831,7 +4831,7 @@
         <v>13</v>
       </c>
       <c r="J56" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="K56" t="s">
         <v>33</v>
@@ -4846,7 +4846,7 @@
         <v>3</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P56" t="s">
         <v>42</v>
@@ -4858,30 +4858,30 @@
         <v>60</v>
       </c>
       <c r="S56" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B57" t="s">
         <v>250</v>
-      </c>
-      <c r="B57" t="s">
-        <v>251</v>
       </c>
       <c r="C57">
         <v>2019</v>
       </c>
       <c r="D57" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E57">
         <v>9.4</v>
       </c>
       <c r="F57" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G57" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H57" t="s">
         <v>38</v>
@@ -4917,33 +4917,33 @@
         <v>59</v>
       </c>
       <c r="S57" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="58" spans="1:19">
-      <c r="A58" s="1" t="s">
+      <c r="B58" t="s">
         <v>255</v>
-      </c>
-      <c r="B58" t="s">
-        <v>256</v>
       </c>
       <c r="C58">
         <v>2019</v>
       </c>
       <c r="D58" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E58">
         <v>7</v>
       </c>
       <c r="F58" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G58" t="s">
         <v>55</v>
       </c>
       <c r="H58" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I58" t="s">
         <v>48</v>
@@ -4964,7 +4964,7 @@
         <v>15</v>
       </c>
       <c r="O58" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P58">
         <v>1</v>
@@ -4976,27 +4976,27 @@
         <v>59</v>
       </c>
       <c r="S58" s="4" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B59" t="s">
         <v>260</v>
-      </c>
-      <c r="B59" t="s">
-        <v>261</v>
       </c>
       <c r="C59">
         <v>2020</v>
       </c>
       <c r="D59" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E59">
         <v>7</v>
       </c>
       <c r="F59" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G59" t="s">
         <v>55</v>
@@ -5014,7 +5014,7 @@
         <v>33</v>
       </c>
       <c r="L59" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="M59" t="s">
         <v>82</v>
@@ -5023,7 +5023,7 @@
         <v>1</v>
       </c>
       <c r="O59" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P59">
         <v>9</v>
@@ -5035,7 +5035,7 @@
         <v>59</v>
       </c>
       <c r="S59" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -5112,14 +5112,14 @@
       <selection activeCell="AJ1" sqref="AJ1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47.1640625" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" customWidth="1"/>
     <col min="27" max="27" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -5136,40 +5136,40 @@
         <v>71</v>
       </c>
       <c r="F1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H1" t="s">
         <v>37</v>
       </c>
       <c r="I1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K1" t="s">
         <v>72</v>
       </c>
       <c r="L1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O1" t="s">
+        <v>131</v>
+      </c>
+      <c r="P1" t="s">
         <v>132</v>
       </c>
-      <c r="P1" t="s">
-        <v>133</v>
-      </c>
       <c r="Q1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="R1" t="s">
         <v>73</v>
@@ -5184,54 +5184,54 @@
         <v>76</v>
       </c>
       <c r="V1" t="s">
+        <v>141</v>
+      </c>
+      <c r="W1" t="s">
         <v>142</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>143</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>144</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>145</v>
       </c>
-      <c r="Z1" t="s">
-        <v>146</v>
-      </c>
       <c r="AA1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AB1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AC1" t="s">
         <v>170</v>
       </c>
-      <c r="AC1" t="s">
-        <v>171</v>
-      </c>
       <c r="AD1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AF1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AG1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AH1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AI1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AJ1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B2">
         <v>0.48999999999999994</v>
@@ -5240,7 +5240,7 @@
         <v>0.70559999999999989</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -5263,9 +5263,9 @@
         <v>0.59289999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B4">
         <v>0.77439999999999998</v>
@@ -5277,7 +5277,7 @@
         <v>0.53290000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>0.64000000000000012</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -5313,15 +5313,15 @@
         <v>0.46240000000000009</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="R8">
         <v>0.73270000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -5341,7 +5341,7 @@
         <v>0.12249999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -5349,7 +5349,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>79</v>
       </c>
@@ -5378,7 +5378,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>84</v>
       </c>
@@ -5386,7 +5386,7 @@
         <v>0.51839999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>88</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>0.6241000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>92</v>
       </c>
@@ -5405,7 +5405,7 @@
         <v>0.33400000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:36">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>98</v>
       </c>
@@ -5416,17 +5416,17 @@
         <v>0.2787</v>
       </c>
     </row>
-    <row r="16" spans="1:36">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="T16">
         <v>0.44890000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C17">
         <v>0.34810000000000002</v>
@@ -5435,7 +5435,7 @@
         <v>0.27039999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>107</v>
       </c>
@@ -5443,23 +5443,23 @@
         <v>0.69499999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D19">
         <v>0.31</v>
       </c>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K20">
         <v>0.98009999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>109</v>
       </c>
@@ -5470,9 +5470,9 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B22">
         <v>0.59289999999999998</v>
@@ -5487,7 +5487,7 @@
         <v>0.34810000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>115</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>0.33800000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>120</v>
       </c>
@@ -5506,9 +5506,9 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K25">
         <v>0.72250000000000003</v>
@@ -5532,9 +5532,9 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B26">
         <v>0.43559999999999999</v>
@@ -5573,17 +5573,17 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="27" spans="1:35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D27">
         <v>7.2900000000000006E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="T28">
         <v>0.36</v>
@@ -5592,17 +5592,17 @@
         <v>0.60840000000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H29">
         <v>0.01</v>
       </c>
     </row>
-    <row r="30" spans="1:35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="R30">
         <v>0.23710000000000001</v>
@@ -5614,25 +5614,25 @@
         <v>0.30690000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K31">
         <v>0.28720000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AA32">
         <v>0.1764</v>
       </c>
     </row>
-    <row r="33" spans="1:36">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="R33">
         <v>0.1197</v>
@@ -5647,9 +5647,9 @@
         <v>0.12959999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:36">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B34">
         <v>0.77</v>
@@ -5670,9 +5670,9 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="35" spans="1:36">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C35">
         <v>0.40960000000000002</v>
@@ -5693,9 +5693,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="36" spans="1:36">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="S36">
         <v>0.1225</v>
@@ -5713,9 +5713,9 @@
         <v>0.33639999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:36">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B37">
         <v>0.27</v>
@@ -5724,9 +5724,9 @@
         <v>0.23499999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:36">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H38">
         <v>0.1444</v>
@@ -5744,9 +5744,9 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:36">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="R39">
         <v>0.19889999999999999</v>
@@ -5761,25 +5761,25 @@
         <v>0.1482</v>
       </c>
     </row>
-    <row r="40" spans="1:36">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D40">
         <v>0.6724</v>
       </c>
     </row>
-    <row r="41" spans="1:36">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K41">
         <v>0.77900000000000003</v>
       </c>
     </row>
-    <row r="42" spans="1:36">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H42">
         <v>0.51690000000000003</v>
@@ -5803,41 +5803,41 @@
         <v>0.55200000000000005</v>
       </c>
     </row>
-    <row r="43" spans="1:36">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H43">
         <v>0.94</v>
       </c>
     </row>
-    <row r="44" spans="1:36">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="R44">
         <v>0.33400000000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:36">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H45">
         <v>0.76680000000000004</v>
       </c>
     </row>
-    <row r="46" spans="1:36">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AE46">
         <v>0.74</v>
       </c>
     </row>
-    <row r="47" spans="1:36">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B47">
         <v>0.33979999999999999</v>
@@ -5849,9 +5849,9 @@
         <v>6.9999999999999999E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:36">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="R48">
         <v>0.31359999999999999</v>
@@ -5875,9 +5875,9 @@
         <v>0.14130000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:34">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="R49">
         <v>0.57069999999999999</v>
@@ -5892,9 +5892,9 @@
         <v>0.19869999999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:34">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D50">
         <v>0.66</v>
@@ -5909,9 +5909,9 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="51" spans="1:34">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="R51">
         <v>0.75690000000000002</v>
@@ -5923,9 +5923,9 @@
         <v>0.82809999999999995</v>
       </c>
     </row>
-    <row r="52" spans="1:34">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="R52">
         <v>0.1024</v>
@@ -5937,9 +5937,9 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:34">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H53">
         <f>0.78</f>
@@ -5949,25 +5949,25 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="54" spans="1:34">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K54">
         <v>0.82</v>
       </c>
     </row>
-    <row r="55" spans="1:34">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R55">
         <v>0.27039999999999997</v>
       </c>
     </row>
-    <row r="56" spans="1:34">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="R56">
         <v>3.61E-2</v>
@@ -5976,9 +5976,9 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="57" spans="1:34">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="R57">
         <v>5.7599999999999998E-2</v>
@@ -5990,9 +5990,9 @@
         <v>3.61E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:34">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D58">
         <v>0.46239999999999998</v>
@@ -6007,9 +6007,9 @@
         <v>0.73960000000000004</v>
       </c>
     </row>
-    <row r="59" spans="1:34">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H59">
         <v>0.46</v>

</xml_diff>